<commit_message>
added footer to stocktaking
</commit_message>
<xml_diff>
--- a/static/inv_tmpl.xlsx
+++ b/static/inv_tmpl.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/crchemist/development/pmm_appdx_47_dev/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B369EB2-5ABC-CA45-AD80-2DFA51384F79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B91A24E-FC92-5F49-84EF-1085F6CEF6FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4300" yWindow="2700" windowWidth="27640" windowHeight="16940" xr2:uid="{091A642D-4557-0E4E-A8B4-0F54D2C62D45}"/>
+    <workbookView xWindow="8200" yWindow="4320" windowWidth="27640" windowHeight="16940" xr2:uid="{091A642D-4557-0E4E-A8B4-0F54D2C62D45}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
   <definedNames>
     <definedName name="Zapasi">[1]pr!$E$34:$E$61</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="54">
   <si>
     <t>запасів</t>
   </si>
@@ -197,12 +197,75 @@
   <si>
     <t xml:space="preserve">вартість </t>
   </si>
+  <si>
+    <t>Наказ Міністерства фінансів України</t>
+  </si>
+  <si>
+    <t>(установа)</t>
+  </si>
+  <si>
+    <t>17.06.2015  № 572</t>
+  </si>
+  <si>
+    <t>Інвентаризаційний опис</t>
+  </si>
+  <si>
+    <t>ЗАТВЕРДЖЕНО</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Разом за описом: </t>
+  </si>
+  <si>
+    <t>(прописом)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Голова комісії:</t>
+  </si>
+  <si>
+    <t>Члени комісії:</t>
+  </si>
+  <si>
+    <t>Усі цінності, пронумеровані в цьому інвентаризаційному описі з №"1" до №"1", перевірені комісією в натурі в моїй присутності та внесені в опис, у зв’язку з чим претензій до інвентаризаційної комісії не маю. Цінності, перелічені в описі, знаходяться на моєму відповідальному зберіганні.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ВІЙСЬКОВА ЧАСТИНА  А4548				</t>
+  </si>
+  <si>
+    <t>sfwdvfwrv</t>
+  </si>
+  <si>
+    <t>xcvfs</t>
+  </si>
+  <si>
+    <t>dddd</t>
+  </si>
+  <si>
+    <t>dfw</t>
+  </si>
+  <si>
+    <t>xvdf</t>
+  </si>
+  <si>
+    <t>svdfb</t>
+  </si>
+  <si>
+    <t>dfg</t>
+  </si>
+  <si>
+    <t>fsargv</t>
+  </si>
+  <si>
+    <t>asdv fgbrbnrsbhtrbn fgbn n h</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="12">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -253,6 +316,32 @@
       <sz val="8"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <name val="Arial Cyr"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Arial Cyr"/>
       <charset val="204"/>
     </font>
   </fonts>
@@ -313,14 +402,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -328,33 +411,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -368,12 +430,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -390,20 +446,99 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -489,7 +624,7 @@
       <sheetName val="na-4"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="0"/>
       <sheetData sheetId="1">
         <row r="34">
           <cell r="E34" t="str">
@@ -638,11 +773,6 @@
             <v>«11» листопада   2023 р.</v>
           </cell>
         </row>
-        <row r="7">
-          <cell r="B7" t="str">
-            <v>10 серпня 2023 року</v>
-          </cell>
-        </row>
         <row r="8">
           <cell r="B8" t="str">
             <v>10 серпня 2023 року</v>
@@ -654,61 +784,61 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
-      <sheetData sheetId="12" refreshError="1"/>
-      <sheetData sheetId="13" refreshError="1"/>
-      <sheetData sheetId="14" refreshError="1"/>
-      <sheetData sheetId="15" refreshError="1"/>
-      <sheetData sheetId="16" refreshError="1"/>
-      <sheetData sheetId="17" refreshError="1"/>
-      <sheetData sheetId="18" refreshError="1"/>
-      <sheetData sheetId="19" refreshError="1"/>
-      <sheetData sheetId="20" refreshError="1"/>
-      <sheetData sheetId="21" refreshError="1"/>
-      <sheetData sheetId="22" refreshError="1"/>
-      <sheetData sheetId="23" refreshError="1"/>
-      <sheetData sheetId="24" refreshError="1"/>
-      <sheetData sheetId="25" refreshError="1"/>
-      <sheetData sheetId="26" refreshError="1"/>
-      <sheetData sheetId="27" refreshError="1"/>
-      <sheetData sheetId="28" refreshError="1"/>
-      <sheetData sheetId="29" refreshError="1"/>
-      <sheetData sheetId="30" refreshError="1"/>
-      <sheetData sheetId="31" refreshError="1"/>
-      <sheetData sheetId="32" refreshError="1"/>
-      <sheetData sheetId="33" refreshError="1"/>
-      <sheetData sheetId="34" refreshError="1"/>
-      <sheetData sheetId="35" refreshError="1"/>
-      <sheetData sheetId="36" refreshError="1"/>
-      <sheetData sheetId="37" refreshError="1"/>
-      <sheetData sheetId="38" refreshError="1"/>
-      <sheetData sheetId="39" refreshError="1"/>
-      <sheetData sheetId="40" refreshError="1"/>
-      <sheetData sheetId="41" refreshError="1"/>
-      <sheetData sheetId="42" refreshError="1"/>
-      <sheetData sheetId="43" refreshError="1"/>
-      <sheetData sheetId="44" refreshError="1"/>
-      <sheetData sheetId="45" refreshError="1"/>
-      <sheetData sheetId="46" refreshError="1"/>
-      <sheetData sheetId="47" refreshError="1"/>
-      <sheetData sheetId="48" refreshError="1"/>
-      <sheetData sheetId="49" refreshError="1"/>
-      <sheetData sheetId="50" refreshError="1"/>
-      <sheetData sheetId="51" refreshError="1"/>
-      <sheetData sheetId="52" refreshError="1"/>
-      <sheetData sheetId="53" refreshError="1"/>
-      <sheetData sheetId="54" refreshError="1"/>
-      <sheetData sheetId="55" refreshError="1"/>
-      <sheetData sheetId="56" refreshError="1"/>
-      <sheetData sheetId="57" refreshError="1"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
+      <sheetData sheetId="18"/>
+      <sheetData sheetId="19"/>
+      <sheetData sheetId="20"/>
+      <sheetData sheetId="21"/>
+      <sheetData sheetId="22"/>
+      <sheetData sheetId="23"/>
+      <sheetData sheetId="24"/>
+      <sheetData sheetId="25"/>
+      <sheetData sheetId="26"/>
+      <sheetData sheetId="27"/>
+      <sheetData sheetId="28"/>
+      <sheetData sheetId="29"/>
+      <sheetData sheetId="30"/>
+      <sheetData sheetId="31"/>
+      <sheetData sheetId="32"/>
+      <sheetData sheetId="33"/>
+      <sheetData sheetId="34"/>
+      <sheetData sheetId="35"/>
+      <sheetData sheetId="36"/>
+      <sheetData sheetId="37"/>
+      <sheetData sheetId="38"/>
+      <sheetData sheetId="39"/>
+      <sheetData sheetId="40"/>
+      <sheetData sheetId="41"/>
+      <sheetData sheetId="42"/>
+      <sheetData sheetId="43"/>
+      <sheetData sheetId="44"/>
+      <sheetData sheetId="45"/>
+      <sheetData sheetId="46"/>
+      <sheetData sheetId="47"/>
+      <sheetData sheetId="48"/>
+      <sheetData sheetId="49"/>
+      <sheetData sheetId="50"/>
+      <sheetData sheetId="51"/>
+      <sheetData sheetId="52"/>
+      <sheetData sheetId="53"/>
+      <sheetData sheetId="54"/>
+      <sheetData sheetId="55"/>
+      <sheetData sheetId="56"/>
+      <sheetData sheetId="57"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1031,104 +1161,101 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3BDDE9D-88C4-E34E-B544-B5F8E71940CE}">
-  <dimension ref="A1:M28"/>
+  <dimension ref="A1:M58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17:G17"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="H57" sqref="H57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
     <row r="1" spans="1:13">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
+      <c r="A1" s="5"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
     </row>
     <row r="2" spans="1:13">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
     </row>
     <row r="3" spans="1:13">
-      <c r="A3" s="2" t="str">
-        <f>[1]Заполнить!$B$6</f>
-        <v>«11» листопада   2023 р.</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
+      <c r="A3" s="46" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="46"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
     </row>
     <row r="4" spans="1:13">
-      <c r="A4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
+      <c r="A4" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="39"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
     </row>
     <row r="5" spans="1:13">
-      <c r="A5" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
     </row>
     <row r="6" spans="1:13">
-      <c r="A6" s="5" t="s">
-        <v>4</v>
-      </c>
+      <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -1143,458 +1270,931 @@
       <c r="M6" s="5"/>
     </row>
     <row r="7" spans="1:13">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
-      <c r="M7" s="6"/>
+      <c r="A7" s="50" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="50"/>
+      <c r="C7" s="50"/>
+      <c r="D7" s="50"/>
+      <c r="E7" s="50"/>
+      <c r="F7" s="50"/>
+      <c r="G7" s="50"/>
+      <c r="H7" s="50"/>
+      <c r="I7" s="50"/>
+      <c r="J7" s="50"/>
+      <c r="K7" s="50"/>
+      <c r="L7" s="50"/>
+      <c r="M7" s="50"/>
     </row>
     <row r="8" spans="1:13">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="50" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="50"/>
+      <c r="C8" s="50"/>
+      <c r="D8" s="50"/>
+      <c r="E8" s="50"/>
+      <c r="F8" s="50"/>
+      <c r="G8" s="50"/>
+      <c r="H8" s="50"/>
+      <c r="I8" s="50"/>
+      <c r="J8" s="50"/>
+      <c r="K8" s="50"/>
+      <c r="L8" s="50"/>
+      <c r="M8" s="50"/>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" s="50" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="50"/>
+      <c r="C9" s="50"/>
+      <c r="D9" s="50"/>
+      <c r="E9" s="50"/>
+      <c r="F9" s="50"/>
+      <c r="G9" s="50"/>
+      <c r="H9" s="50"/>
+      <c r="I9" s="50"/>
+      <c r="J9" s="50"/>
+      <c r="K9" s="50"/>
+      <c r="L9" s="50"/>
+      <c r="M9" s="50"/>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" s="51" t="str">
+        <f>[1]Заполнить!$B$6</f>
+        <v>«11» листопада   2023 р.</v>
+      </c>
+      <c r="B10" s="51"/>
+      <c r="C10" s="51"/>
+      <c r="D10" s="51"/>
+      <c r="E10" s="51"/>
+      <c r="F10" s="51"/>
+      <c r="G10" s="51"/>
+      <c r="H10" s="51"/>
+      <c r="I10" s="51"/>
+      <c r="J10" s="51"/>
+      <c r="K10" s="51"/>
+      <c r="L10" s="51"/>
+      <c r="M10" s="51"/>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="39"/>
+      <c r="C11" s="39"/>
+      <c r="D11" s="39"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
+      <c r="G11" s="39"/>
+      <c r="H11" s="39"/>
+      <c r="I11" s="39"/>
+      <c r="J11" s="39"/>
+      <c r="K11" s="39"/>
+      <c r="L11" s="39"/>
+      <c r="M11" s="39"/>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" s="52" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="52"/>
+      <c r="C12" s="52"/>
+      <c r="D12" s="52"/>
+      <c r="E12" s="52"/>
+      <c r="F12" s="52"/>
+      <c r="G12" s="52"/>
+      <c r="H12" s="52"/>
+      <c r="I12" s="52"/>
+      <c r="J12" s="52"/>
+      <c r="K12" s="52"/>
+      <c r="L12" s="52"/>
+      <c r="M12" s="52"/>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="49"/>
+      <c r="C13" s="49"/>
+      <c r="D13" s="49"/>
+      <c r="E13" s="49"/>
+      <c r="F13" s="49"/>
+      <c r="G13" s="49"/>
+      <c r="H13" s="49"/>
+      <c r="I13" s="49"/>
+      <c r="J13" s="49"/>
+      <c r="K13" s="49"/>
+      <c r="L13" s="49"/>
+      <c r="M13" s="49"/>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" s="38"/>
+      <c r="B14" s="38"/>
+      <c r="C14" s="38"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="38"/>
+      <c r="J14" s="38"/>
+      <c r="K14" s="38"/>
+      <c r="L14" s="38"/>
+      <c r="M14" s="38"/>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-    </row>
-    <row r="9" spans="1:13">
-      <c r="A9" s="7" t="s">
+      <c r="B15" s="39"/>
+      <c r="C15" s="39"/>
+      <c r="D15" s="39"/>
+      <c r="E15" s="39"/>
+      <c r="F15" s="39"/>
+      <c r="G15" s="39"/>
+      <c r="H15" s="39"/>
+      <c r="I15" s="39"/>
+      <c r="J15" s="39"/>
+      <c r="K15" s="39"/>
+      <c r="L15" s="39"/>
+      <c r="M15" s="39"/>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="A16" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="8" t="s">
+      <c r="B16" s="3"/>
+      <c r="C16" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="8"/>
-    </row>
-    <row r="10" spans="1:13">
-      <c r="A10" s="9"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="3" t="s">
+      <c r="D16" s="47"/>
+      <c r="E16" s="47"/>
+      <c r="F16" s="47"/>
+      <c r="G16" s="47"/>
+      <c r="H16" s="47"/>
+      <c r="I16" s="47"/>
+      <c r="J16" s="47"/>
+      <c r="K16" s="47"/>
+      <c r="L16" s="47"/>
+      <c r="M16" s="47"/>
+    </row>
+    <row r="17" spans="1:13" ht="16" customHeight="1">
+      <c r="A17" s="4"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
-    </row>
-    <row r="11" spans="1:13">
-      <c r="A11" s="11" t="str">
-        <f>CONCATENATE("станом на ",[1]Заполнить!$B$7)</f>
-        <v>станом на 10 серпня 2023 року</v>
-      </c>
-      <c r="B11" s="11"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
-      <c r="K11" s="12"/>
-      <c r="L11" s="12"/>
-      <c r="M11" s="12"/>
-    </row>
-    <row r="12" spans="1:13">
-      <c r="A12" s="12"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12"/>
-      <c r="K12" s="12"/>
-      <c r="L12" s="12"/>
-      <c r="M12" s="12"/>
-    </row>
-    <row r="13" spans="1:13">
-      <c r="A13" s="13" t="s">
+      <c r="D17" s="39"/>
+      <c r="E17" s="39"/>
+      <c r="F17" s="39"/>
+      <c r="G17" s="39"/>
+      <c r="H17" s="39"/>
+      <c r="I17" s="39"/>
+      <c r="J17" s="39"/>
+      <c r="K17" s="39"/>
+      <c r="L17" s="39"/>
+      <c r="M17" s="39"/>
+    </row>
+    <row r="18" spans="1:13">
+      <c r="A18" s="48" t="str">
+        <f>CONCATENATE("станом на ","10 cthgyz")</f>
+        <v>станом на 10 cthgyz</v>
+      </c>
+      <c r="B18" s="48"/>
+      <c r="C18" s="48"/>
+      <c r="D18" s="48"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5"/>
+      <c r="M18" s="5"/>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="5"/>
+      <c r="M19" s="5"/>
+    </row>
+    <row r="20" spans="1:13">
+      <c r="A20" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="13"/>
-      <c r="K13" s="13"/>
-      <c r="L13" s="13"/>
-      <c r="M13" s="13"/>
-    </row>
-    <row r="14" spans="1:13">
-      <c r="A14" s="14" t="s">
+      <c r="B20" s="41"/>
+      <c r="C20" s="41"/>
+      <c r="D20" s="41"/>
+      <c r="E20" s="41"/>
+      <c r="F20" s="41"/>
+      <c r="G20" s="41"/>
+      <c r="H20" s="41"/>
+      <c r="I20" s="41"/>
+      <c r="J20" s="41"/>
+      <c r="K20" s="41"/>
+      <c r="L20" s="41"/>
+      <c r="M20" s="41"/>
+    </row>
+    <row r="21" spans="1:13">
+      <c r="A21" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="14"/>
-      <c r="L14" s="14"/>
-      <c r="M14" s="14"/>
-    </row>
-    <row r="15" spans="1:13">
-      <c r="A15" s="14"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="14"/>
-      <c r="M15" s="14"/>
-    </row>
-    <row r="16" spans="1:13">
-      <c r="A16" s="15"/>
-      <c r="B16" s="15"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="15"/>
-      <c r="I16" s="15"/>
-      <c r="J16" s="15"/>
-      <c r="K16" s="15"/>
-      <c r="L16" s="12"/>
-      <c r="M16" s="12"/>
-    </row>
-    <row r="17" spans="1:13">
-      <c r="A17" s="16" t="s">
+      <c r="B21" s="42"/>
+      <c r="C21" s="42"/>
+      <c r="D21" s="42"/>
+      <c r="E21" s="42"/>
+      <c r="F21" s="42"/>
+      <c r="G21" s="42"/>
+      <c r="H21" s="42"/>
+      <c r="I21" s="42"/>
+      <c r="J21" s="42"/>
+      <c r="K21" s="42"/>
+      <c r="L21" s="42"/>
+      <c r="M21" s="42"/>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="A22" s="42"/>
+      <c r="B22" s="42"/>
+      <c r="C22" s="42"/>
+      <c r="D22" s="42"/>
+      <c r="E22" s="42"/>
+      <c r="F22" s="42"/>
+      <c r="G22" s="42"/>
+      <c r="H22" s="42"/>
+      <c r="I22" s="42"/>
+      <c r="J22" s="42"/>
+      <c r="K22" s="42"/>
+      <c r="L22" s="42"/>
+      <c r="M22" s="42"/>
+    </row>
+    <row r="23" spans="1:13">
+      <c r="A23" s="6"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="5"/>
+    </row>
+    <row r="24" spans="1:13">
+      <c r="A24" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="12"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="18" t="s">
+      <c r="B24" s="5"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="15"/>
-      <c r="I17" s="19"/>
-      <c r="J17" s="15"/>
-      <c r="K17" s="20" t="s">
+      <c r="E24" s="43"/>
+      <c r="F24" s="43"/>
+      <c r="G24" s="43"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="10"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="L17" s="20"/>
-      <c r="M17" s="20"/>
-    </row>
-    <row r="18" spans="1:13">
-      <c r="A18" s="21"/>
-      <c r="B18" s="21"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="22" t="s">
+      <c r="L24" s="44"/>
+      <c r="M24" s="44"/>
+    </row>
+    <row r="25" spans="1:13" ht="16" customHeight="1">
+      <c r="A25" s="11"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="E18" s="22"/>
-      <c r="F18" s="22"/>
-      <c r="G18" s="22"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="10" t="s">
+      <c r="E25" s="45"/>
+      <c r="F25" s="45"/>
+      <c r="G25" s="45"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J18" s="21"/>
-      <c r="K18" s="3" t="s">
+      <c r="J25" s="11"/>
+      <c r="K25" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="L18" s="3"/>
-      <c r="M18" s="3"/>
-    </row>
-    <row r="19" spans="1:13">
-      <c r="A19" s="12"/>
-      <c r="B19" s="15"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="15"/>
-      <c r="H19" s="15"/>
-      <c r="I19" s="15"/>
-      <c r="J19" s="15"/>
-      <c r="K19" s="15"/>
-      <c r="L19" s="12"/>
-      <c r="M19" s="12"/>
-    </row>
-    <row r="20" spans="1:13">
-      <c r="A20" s="16" t="s">
+      <c r="L25" s="39"/>
+      <c r="M25" s="39"/>
+    </row>
+    <row r="26" spans="1:13">
+      <c r="A26" s="5"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="6"/>
+      <c r="K26" s="6"/>
+      <c r="L26" s="5"/>
+      <c r="M26" s="5"/>
+    </row>
+    <row r="27" spans="1:13">
+      <c r="A27" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="15"/>
-      <c r="C20" s="23" t="str">
+      <c r="B27" s="6"/>
+      <c r="C27" s="12" t="str">
         <f>CONCATENATE("розпочата ",[1]Заполнить!$B$8)</f>
         <v>розпочата 10 серпня 2023 року</v>
       </c>
-      <c r="D20" s="15"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="15"/>
-      <c r="H20" s="15"/>
-      <c r="I20" s="15"/>
-      <c r="J20" s="15"/>
-      <c r="K20" s="15"/>
-      <c r="L20" s="12"/>
-      <c r="M20" s="12"/>
-    </row>
-    <row r="21" spans="1:13">
-      <c r="A21" s="15"/>
-      <c r="B21" s="15"/>
-      <c r="C21" s="16" t="str">
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="6"/>
+      <c r="K27" s="6"/>
+      <c r="L27" s="5"/>
+      <c r="M27" s="5"/>
+    </row>
+    <row r="28" spans="1:13" ht="16" customHeight="1">
+      <c r="A28" s="6"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="7" t="str">
         <f>CONCATENATE("закінчена ",[1]Заполнить!$B$9)</f>
         <v>закінчена 20 серпня 2023 року</v>
       </c>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="15"/>
-      <c r="H21" s="15"/>
-      <c r="I21" s="15"/>
-      <c r="J21" s="15"/>
-      <c r="K21" s="15"/>
-      <c r="L21" s="12"/>
-      <c r="M21" s="12"/>
-    </row>
-    <row r="22" spans="1:13">
-      <c r="A22" s="15"/>
-      <c r="B22" s="15"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="15"/>
-      <c r="I22" s="15"/>
-      <c r="J22" s="15"/>
-      <c r="K22" s="15"/>
-      <c r="L22" s="12"/>
-      <c r="M22" s="12"/>
-    </row>
-    <row r="23" spans="1:13">
-      <c r="A23" s="24"/>
-      <c r="B23" s="12"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
-      <c r="H23" s="12"/>
-      <c r="I23" s="12"/>
-      <c r="J23" s="12"/>
-      <c r="K23" s="12"/>
-      <c r="L23" s="12"/>
-      <c r="M23" s="12"/>
-    </row>
-    <row r="24" spans="1:13">
-      <c r="A24" s="25" t="s">
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="6"/>
+      <c r="J28" s="6"/>
+      <c r="K28" s="6"/>
+      <c r="L28" s="5"/>
+      <c r="M28" s="5"/>
+    </row>
+    <row r="29" spans="1:13">
+      <c r="A29" s="6"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="6"/>
+      <c r="K29" s="6"/>
+      <c r="L29" s="5"/>
+      <c r="M29" s="5"/>
+    </row>
+    <row r="30" spans="1:13">
+      <c r="A30" s="13"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="5"/>
+      <c r="J30" s="5"/>
+      <c r="K30" s="5"/>
+      <c r="L30" s="5"/>
+      <c r="M30" s="5"/>
+    </row>
+    <row r="31" spans="1:13">
+      <c r="A31" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="B24" s="12"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="12"/>
-      <c r="H24" s="12"/>
-      <c r="I24" s="12"/>
-      <c r="J24" s="12"/>
-      <c r="K24" s="12"/>
-      <c r="L24" s="12"/>
-      <c r="M24" s="12"/>
-    </row>
-    <row r="25" spans="1:13">
-      <c r="A25" s="12" t="s">
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
+      <c r="I31" s="5"/>
+      <c r="J31" s="5"/>
+      <c r="K31" s="5"/>
+      <c r="L31" s="5"/>
+      <c r="M31" s="5"/>
+    </row>
+    <row r="32" spans="1:13">
+      <c r="A32" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B25" s="12"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
-      <c r="G25" s="12"/>
-      <c r="H25" s="12"/>
-      <c r="I25" s="12"/>
-      <c r="J25" s="12"/>
-      <c r="K25" s="12"/>
-      <c r="L25" s="12"/>
-      <c r="M25" s="12"/>
-    </row>
-    <row r="26" spans="1:13">
-      <c r="A26" s="26" t="s">
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
+      <c r="I32" s="5"/>
+      <c r="J32" s="5"/>
+      <c r="K32" s="5"/>
+      <c r="L32" s="5"/>
+      <c r="M32" s="5"/>
+    </row>
+    <row r="33" spans="1:13">
+      <c r="A33" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="B26" s="26" t="s">
+      <c r="B33" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="C26" s="26" t="s">
+      <c r="C33" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="D26" s="26"/>
-      <c r="E26" s="27" t="s">
+      <c r="D33" s="36"/>
+      <c r="E33" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="F26" s="26" t="s">
+      <c r="F33" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="G26" s="26"/>
-      <c r="H26" s="26"/>
-      <c r="I26" s="26" t="s">
+      <c r="G33" s="36"/>
+      <c r="H33" s="36"/>
+      <c r="I33" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="J26" s="26"/>
-      <c r="K26" s="26"/>
-      <c r="L26" s="26" t="s">
+      <c r="J33" s="36"/>
+      <c r="K33" s="36"/>
+      <c r="L33" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="M26" s="26"/>
-    </row>
-    <row r="27" spans="1:13" ht="51">
-      <c r="A27" s="26"/>
-      <c r="B27" s="26"/>
-      <c r="C27" s="28" t="s">
+      <c r="M33" s="36"/>
+    </row>
+    <row r="34" spans="1:13" ht="51">
+      <c r="A34" s="36"/>
+      <c r="B34" s="36"/>
+      <c r="C34" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="D27" s="29" t="s">
+      <c r="D34" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="E27" s="27"/>
-      <c r="F27" s="28" t="s">
+      <c r="E34" s="40"/>
+      <c r="F34" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="G27" s="28" t="s">
+      <c r="G34" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="H27" s="28" t="s">
+      <c r="H34" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="I27" s="28" t="s">
+      <c r="I34" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="J27" s="28" t="s">
+      <c r="J34" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="K27" s="28" t="s">
+      <c r="K34" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="L27" s="26"/>
-      <c r="M27" s="26"/>
-    </row>
-    <row r="28" spans="1:13">
-      <c r="A28" s="30">
+      <c r="L34" s="36"/>
+      <c r="M34" s="36"/>
+    </row>
+    <row r="35" spans="1:13">
+      <c r="A35" s="17">
         <v>1</v>
       </c>
-      <c r="B28" s="30">
+      <c r="B35" s="17">
         <v>2</v>
       </c>
-      <c r="C28" s="30">
+      <c r="C35" s="17">
         <v>3</v>
       </c>
-      <c r="D28" s="30">
+      <c r="D35" s="17">
         <v>4</v>
       </c>
-      <c r="E28" s="30">
+      <c r="E35" s="17">
         <v>5</v>
       </c>
-      <c r="F28" s="31">
+      <c r="F35" s="18">
         <v>6</v>
       </c>
-      <c r="G28" s="30">
+      <c r="G35" s="17">
         <v>7</v>
       </c>
-      <c r="H28" s="30">
+      <c r="H35" s="17">
         <v>8</v>
       </c>
-      <c r="I28" s="30">
+      <c r="I35" s="17">
         <v>9</v>
       </c>
-      <c r="J28" s="30">
+      <c r="J35" s="17">
         <v>10</v>
       </c>
-      <c r="K28" s="30">
+      <c r="K35" s="17">
         <v>11</v>
       </c>
-      <c r="L28" s="32">
+      <c r="L35" s="37">
         <v>12</v>
       </c>
-      <c r="M28" s="32"/>
+      <c r="M35" s="37"/>
+    </row>
+    <row r="39" spans="1:13">
+      <c r="A39" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B39" s="5"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
+      <c r="G39" s="5"/>
+      <c r="H39" s="5"/>
+      <c r="I39" s="5"/>
+      <c r="J39" s="5"/>
+      <c r="K39" s="5"/>
+      <c r="L39" s="5"/>
+      <c r="M39" s="5"/>
+    </row>
+    <row r="40" spans="1:13">
+      <c r="A40" s="5"/>
+      <c r="B40" s="5"/>
+      <c r="D40" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E40" s="5"/>
+      <c r="F40" s="5"/>
+      <c r="G40" s="5"/>
+      <c r="H40" s="5"/>
+      <c r="I40" s="5"/>
+      <c r="J40" s="5"/>
+      <c r="K40" s="5"/>
+      <c r="L40" s="5"/>
+      <c r="M40" s="5"/>
+    </row>
+    <row r="41" spans="1:13">
+      <c r="A41" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="B41" s="5"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="7"/>
+      <c r="F41" s="5"/>
+      <c r="G41" s="5"/>
+      <c r="H41" s="5"/>
+      <c r="I41" s="5"/>
+      <c r="J41" s="5"/>
+      <c r="K41" s="5"/>
+      <c r="L41" s="5"/>
+      <c r="M41" s="5"/>
+    </row>
+    <row r="42" spans="1:13">
+      <c r="A42" s="5"/>
+      <c r="B42" s="5"/>
+      <c r="D42" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E42" s="14"/>
+      <c r="F42" s="14"/>
+      <c r="G42" s="5"/>
+      <c r="H42" s="5"/>
+      <c r="I42" s="5"/>
+      <c r="J42" s="5"/>
+      <c r="K42" s="5"/>
+      <c r="L42" s="5"/>
+      <c r="M42" s="5"/>
+    </row>
+    <row r="43" spans="1:13">
+      <c r="A43" s="5"/>
+      <c r="B43" s="5"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="3"/>
+      <c r="G43" s="3"/>
+      <c r="H43" s="3"/>
+      <c r="I43" s="3"/>
+      <c r="J43" s="3"/>
+      <c r="K43" s="5"/>
+      <c r="L43" s="5"/>
+      <c r="M43" s="5"/>
+    </row>
+    <row r="44" spans="1:13">
+      <c r="A44" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="B44" s="5"/>
+      <c r="C44" s="7"/>
+      <c r="D44" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E44" s="5"/>
+      <c r="F44" s="5"/>
+      <c r="G44" s="5"/>
+      <c r="H44" s="5"/>
+      <c r="I44" s="5"/>
+      <c r="J44" s="5"/>
+      <c r="K44" s="5"/>
+      <c r="L44" s="5"/>
+      <c r="M44" s="5"/>
+    </row>
+    <row r="45" spans="1:13">
+      <c r="A45" s="22"/>
+      <c r="B45" s="5"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="14"/>
+      <c r="E45" s="5"/>
+      <c r="F45" s="5"/>
+      <c r="G45" s="5"/>
+      <c r="H45" s="5"/>
+      <c r="I45" s="5"/>
+      <c r="J45" s="5"/>
+      <c r="K45" s="5"/>
+      <c r="L45" s="5"/>
+      <c r="M45" s="5"/>
+    </row>
+    <row r="46" spans="1:13" ht="16" customHeight="1">
+      <c r="A46" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="C46" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="D46" s="33"/>
+      <c r="E46" s="33"/>
+      <c r="F46" s="33"/>
+      <c r="G46" s="33"/>
+      <c r="H46" s="24"/>
+      <c r="I46" s="25"/>
+      <c r="J46" s="24"/>
+      <c r="K46" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="L46" s="30"/>
+      <c r="M46" s="30"/>
+    </row>
+    <row r="47" spans="1:13">
+      <c r="D47" s="14"/>
+      <c r="E47" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="F47" s="14"/>
+      <c r="G47" s="14"/>
+      <c r="H47" s="26"/>
+      <c r="I47" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J47" s="26"/>
+      <c r="L47" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="M47" s="14"/>
+    </row>
+    <row r="48" spans="1:13" ht="16" customHeight="1">
+      <c r="A48" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="C48" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="D48" s="33"/>
+      <c r="E48" s="33"/>
+      <c r="F48" s="33"/>
+      <c r="G48" s="33"/>
+      <c r="H48" s="24"/>
+      <c r="I48" s="25"/>
+      <c r="J48" s="24"/>
+      <c r="K48" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="L48" s="30"/>
+      <c r="M48" s="30"/>
+    </row>
+    <row r="49" spans="1:13">
+      <c r="D49" s="14"/>
+      <c r="E49" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F49" s="14"/>
+      <c r="G49" s="14"/>
+      <c r="H49" s="26"/>
+      <c r="I49" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J49" s="26"/>
+      <c r="L49" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="M49" s="14"/>
+    </row>
+    <row r="50" spans="1:13" ht="16" customHeight="1">
+      <c r="C50" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="D50" s="33"/>
+      <c r="E50" s="33"/>
+      <c r="F50" s="33"/>
+      <c r="G50" s="33"/>
+      <c r="H50" s="24"/>
+      <c r="I50" s="25"/>
+      <c r="J50" s="24"/>
+      <c r="K50" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="L50" s="30"/>
+      <c r="M50" s="30"/>
+    </row>
+    <row r="51" spans="1:13">
+      <c r="D51" s="14"/>
+      <c r="E51" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F51" s="14"/>
+      <c r="G51" s="14"/>
+      <c r="H51" s="26"/>
+      <c r="I51" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J51" s="26"/>
+      <c r="L51" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="M51" s="14"/>
+    </row>
+    <row r="52" spans="1:13" ht="16" customHeight="1">
+      <c r="A52" s="27"/>
+      <c r="B52" s="27"/>
+      <c r="C52" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="D52" s="32"/>
+      <c r="E52" s="32"/>
+      <c r="F52" s="32"/>
+      <c r="G52" s="32"/>
+      <c r="H52" s="24"/>
+      <c r="I52" s="28"/>
+      <c r="J52" s="24"/>
+      <c r="K52" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="L52" s="31"/>
+      <c r="M52" s="31"/>
+    </row>
+    <row r="53" spans="1:13">
+      <c r="A53" s="27"/>
+      <c r="B53" s="27"/>
+      <c r="D53" s="14"/>
+      <c r="E53" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F53" s="14"/>
+      <c r="G53" s="14"/>
+      <c r="H53" s="26"/>
+      <c r="I53" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J53" s="26"/>
+      <c r="L53" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="M53" s="14"/>
+    </row>
+    <row r="54" spans="1:13" ht="36" customHeight="1">
+      <c r="A54" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="B54" s="29"/>
+      <c r="C54" s="29"/>
+      <c r="D54" s="29"/>
+      <c r="E54" s="29"/>
+      <c r="F54" s="29"/>
+      <c r="G54" s="29"/>
+      <c r="H54" s="29"/>
+      <c r="I54" s="29"/>
+      <c r="J54" s="29"/>
+      <c r="K54" s="29"/>
+      <c r="L54" s="29"/>
+      <c r="M54" s="29"/>
+    </row>
+    <row r="55" spans="1:13">
+      <c r="A55" s="29"/>
+      <c r="B55" s="29"/>
+      <c r="C55" s="29"/>
+      <c r="D55" s="29"/>
+      <c r="E55" s="29"/>
+      <c r="F55" s="29"/>
+      <c r="G55" s="29"/>
+      <c r="H55" s="29"/>
+      <c r="I55" s="29"/>
+      <c r="J55" s="29"/>
+      <c r="K55" s="29"/>
+      <c r="L55" s="29"/>
+      <c r="M55" s="29"/>
+    </row>
+    <row r="56" spans="1:13">
+      <c r="A56" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B56" s="5"/>
+      <c r="C56" s="5"/>
+      <c r="D56" s="5"/>
+      <c r="E56" s="5"/>
+      <c r="F56" s="5"/>
+      <c r="G56" s="5"/>
+      <c r="H56" s="5"/>
+      <c r="I56" s="5"/>
+      <c r="J56" s="5"/>
+      <c r="K56" s="5"/>
+      <c r="L56" s="5"/>
+      <c r="M56" s="5"/>
+    </row>
+    <row r="57" spans="1:13">
+      <c r="A57" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="B57" s="5"/>
+      <c r="C57" s="5"/>
+      <c r="D57" s="35" t="str">
+        <f>D24</f>
+        <v>командир медичного взводу</v>
+      </c>
+      <c r="F57" s="35"/>
+      <c r="G57" s="2"/>
+      <c r="H57" s="9"/>
+      <c r="I57" s="2"/>
+      <c r="K57" s="35" t="str">
+        <f>K24</f>
+        <v>Г.КОЗАЧЕНКО</v>
+      </c>
+      <c r="L57" s="35"/>
+      <c r="M57" s="35"/>
+    </row>
+    <row r="58" spans="1:13">
+      <c r="A58" s="5"/>
+      <c r="B58" s="5"/>
+      <c r="C58" s="5"/>
+      <c r="E58" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F58" s="14"/>
+      <c r="G58" s="5"/>
+      <c r="H58" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I58" s="5"/>
+      <c r="K58" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="L58" s="14"/>
+      <c r="M58" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="25">
-    <mergeCell ref="I26:K26"/>
-    <mergeCell ref="L26:M27"/>
-    <mergeCell ref="L28:M28"/>
-    <mergeCell ref="A14:M15"/>
-    <mergeCell ref="D17:G17"/>
-    <mergeCell ref="K17:M17"/>
-    <mergeCell ref="D18:G18"/>
-    <mergeCell ref="K18:M18"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="F26:H26"/>
+  <mergeCells count="28">
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="C16:M16"/>
+    <mergeCell ref="C17:M17"/>
+    <mergeCell ref="A18:D18"/>
+    <mergeCell ref="A13:M13"/>
+    <mergeCell ref="A9:M9"/>
+    <mergeCell ref="A10:M10"/>
+    <mergeCell ref="A11:M11"/>
+    <mergeCell ref="A12:M12"/>
     <mergeCell ref="A7:M7"/>
     <mergeCell ref="A8:M8"/>
-    <mergeCell ref="C9:M9"/>
-    <mergeCell ref="C10:M10"/>
-    <mergeCell ref="A11:D11"/>
-    <mergeCell ref="A13:M13"/>
-    <mergeCell ref="A1:M1"/>
-    <mergeCell ref="A2:M2"/>
-    <mergeCell ref="A3:M3"/>
-    <mergeCell ref="A4:M4"/>
-    <mergeCell ref="A5:M5"/>
-    <mergeCell ref="A6:M6"/>
+    <mergeCell ref="I33:K33"/>
+    <mergeCell ref="L33:M34"/>
+    <mergeCell ref="L35:M35"/>
+    <mergeCell ref="A14:M14"/>
+    <mergeCell ref="A15:M15"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="F33:H33"/>
+    <mergeCell ref="A20:M20"/>
+    <mergeCell ref="A21:M22"/>
+    <mergeCell ref="D24:G24"/>
+    <mergeCell ref="K24:M24"/>
+    <mergeCell ref="D25:G25"/>
+    <mergeCell ref="K25:M25"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A7:M7" xr:uid="{AA25D106-1396-8C4A-8DB7-30A8202DC554}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A14:M14" xr:uid="{81B76744-CFBE-2747-9447-E2C34822F190}">
       <formula1>Zapasi</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>